<commit_message>
The same that the last one
</commit_message>
<xml_diff>
--- a/general.xlsx
+++ b/general.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/danny_jimenez_estudiantec_cr/Documents/Extra Job - 2022/Final Project AV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1FD65AA7-57D2-4301-971B-EBF5A6F965A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB18DC6C-1634-0341-86A5-87125B81246F}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{1FD65AA7-57D2-4301-971B-EBF5A6F965A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B573D0D-B46F-EA47-B579-7C67632D976D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40849,7 +40849,7 @@
   <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40859,7 +40859,7 @@
     <col min="3" max="3" width="8.83203125" style="6" customWidth="1"/>
     <col min="4" max="5" width="9.83203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
     <col min="8" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
@@ -40882,7 +40882,7 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -40905,7 +40905,7 @@
       <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="7"/>
@@ -40929,7 +40929,7 @@
       <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="8"/>
@@ -40953,7 +40953,7 @@
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="8"/>
@@ -40977,7 +40977,7 @@
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="8"/>
@@ -41001,7 +41001,7 @@
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="8"/>
@@ -41025,7 +41025,7 @@
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="8"/>
@@ -41049,7 +41049,7 @@
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="8"/>
@@ -41073,7 +41073,7 @@
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="8"/>
@@ -41097,7 +41097,7 @@
       <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="8"/>
@@ -41121,7 +41121,7 @@
       <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="8"/>
@@ -41145,7 +41145,7 @@
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="8"/>
@@ -41169,7 +41169,7 @@
       <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="8"/>
@@ -41193,7 +41193,7 @@
       <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="8"/>
@@ -41217,7 +41217,7 @@
       <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="8"/>
@@ -41241,7 +41241,7 @@
       <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="8"/>
@@ -41265,7 +41265,7 @@
       <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="8"/>
@@ -41289,7 +41289,7 @@
       <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="8"/>
@@ -41313,7 +41313,7 @@
       <c r="F19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="8"/>
@@ -41337,7 +41337,7 @@
       <c r="F20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" t="s">
         <v>28</v>
       </c>
       <c r="H20" s="8"/>
@@ -41361,7 +41361,7 @@
       <c r="F21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" t="s">
         <v>29</v>
       </c>
       <c r="H21" s="8"/>
@@ -41385,7 +41385,7 @@
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" t="s">
         <v>30</v>
       </c>
       <c r="H22" s="8"/>
@@ -41409,7 +41409,7 @@
       <c r="F23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" t="s">
         <v>31</v>
       </c>
       <c r="H23" s="8"/>
@@ -41433,7 +41433,7 @@
       <c r="F24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" t="s">
         <v>32</v>
       </c>
       <c r="H24" s="8"/>
@@ -41457,7 +41457,7 @@
       <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" t="s">
         <v>33</v>
       </c>
       <c r="H25" s="8"/>
@@ -41481,7 +41481,7 @@
       <c r="F26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" t="s">
         <v>34</v>
       </c>
       <c r="H26" s="8"/>
@@ -41505,7 +41505,7 @@
       <c r="F27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="8"/>
@@ -41529,7 +41529,7 @@
       <c r="F28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" t="s">
         <v>36</v>
       </c>
       <c r="H28" s="8"/>
@@ -41553,7 +41553,7 @@
       <c r="F29" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
       <c r="H29" s="8"/>
@@ -41577,7 +41577,7 @@
       <c r="F30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" t="s">
         <v>38</v>
       </c>
       <c r="H30" s="8"/>
@@ -41601,7 +41601,7 @@
       <c r="F31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" t="s">
         <v>39</v>
       </c>
       <c r="H31" s="8"/>
@@ -41625,7 +41625,7 @@
       <c r="F32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" t="s">
         <v>40</v>
       </c>
       <c r="H32" s="8"/>
@@ -41649,7 +41649,7 @@
       <c r="F33" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" t="s">
         <v>41</v>
       </c>
       <c r="H33" s="8"/>
@@ -41673,7 +41673,7 @@
       <c r="F34" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" t="s">
         <v>42</v>
       </c>
       <c r="H34" s="8"/>
@@ -41697,7 +41697,7 @@
       <c r="F35" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" t="s">
         <v>43</v>
       </c>
       <c r="H35" s="8"/>
@@ -41721,7 +41721,7 @@
       <c r="F36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" t="s">
         <v>44</v>
       </c>
       <c r="H36" s="8"/>
@@ -41745,7 +41745,7 @@
       <c r="F37" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" t="s">
         <v>45</v>
       </c>
       <c r="H37" s="8"/>
@@ -41769,7 +41769,7 @@
       <c r="F38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" t="s">
         <v>46</v>
       </c>
       <c r="H38" s="8"/>
@@ -41793,7 +41793,7 @@
       <c r="F39" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G39" t="s">
         <v>47</v>
       </c>
       <c r="H39" s="8"/>
@@ -41817,7 +41817,7 @@
       <c r="F40" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" t="s">
         <v>48</v>
       </c>
       <c r="H40" s="8"/>
@@ -41841,7 +41841,7 @@
       <c r="F41" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" t="s">
         <v>49</v>
       </c>
       <c r="H41" s="8"/>
@@ -41865,7 +41865,7 @@
       <c r="F42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" t="s">
         <v>50</v>
       </c>
       <c r="H42" s="8"/>
@@ -41889,7 +41889,7 @@
       <c r="F43" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" t="s">
         <v>51</v>
       </c>
       <c r="H43" s="8"/>
@@ -41913,7 +41913,7 @@
       <c r="F44" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G44" t="s">
         <v>52</v>
       </c>
       <c r="H44" s="8"/>
@@ -41937,7 +41937,7 @@
       <c r="F45" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G45" t="s">
         <v>53</v>
       </c>
       <c r="H45" s="8"/>
@@ -41961,7 +41961,7 @@
       <c r="F46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G46" t="s">
         <v>54</v>
       </c>
       <c r="H46" s="8"/>
@@ -41985,7 +41985,7 @@
       <c r="F47" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="G47" t="s">
         <v>55</v>
       </c>
       <c r="H47" s="8"/>
@@ -42009,7 +42009,7 @@
       <c r="F48" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G48" t="s">
         <v>56</v>
       </c>
       <c r="H48" s="8"/>
@@ -42033,7 +42033,7 @@
       <c r="F49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" t="s">
         <v>57</v>
       </c>
       <c r="H49" s="8"/>
@@ -42057,7 +42057,7 @@
       <c r="F50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G50" t="s">
         <v>58</v>
       </c>
       <c r="H50" s="8"/>
@@ -42081,7 +42081,7 @@
       <c r="F51" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="G51" t="s">
         <v>59</v>
       </c>
       <c r="H51" s="8"/>
@@ -42105,7 +42105,7 @@
       <c r="F52" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="G52" t="s">
         <v>60</v>
       </c>
       <c r="H52" s="8"/>
@@ -42129,7 +42129,7 @@
       <c r="F53" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="G53" t="s">
         <v>61</v>
       </c>
       <c r="H53" s="8"/>
@@ -42153,7 +42153,7 @@
       <c r="F54" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="G54" t="s">
         <v>62</v>
       </c>
       <c r="H54" s="8"/>
@@ -42177,7 +42177,7 @@
       <c r="F55" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="G55" t="s">
         <v>63</v>
       </c>
       <c r="H55" s="8"/>
@@ -42201,7 +42201,7 @@
       <c r="F56" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G56" t="s">
         <v>64</v>
       </c>
       <c r="H56" s="8"/>
@@ -42225,7 +42225,7 @@
       <c r="F57" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" t="s">
         <v>65</v>
       </c>
       <c r="H57" s="8"/>
@@ -42249,7 +42249,7 @@
       <c r="F58" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="G58" t="s">
         <v>66</v>
       </c>
       <c r="H58" s="8"/>
@@ -42273,7 +42273,7 @@
       <c r="F59" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="G59" t="s">
         <v>67</v>
       </c>
       <c r="H59" s="8"/>
@@ -42297,7 +42297,7 @@
       <c r="F60" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="G60" t="s">
         <v>68</v>
       </c>
       <c r="H60" s="8"/>
@@ -42321,7 +42321,7 @@
       <c r="F61" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="G61" t="s">
         <v>69</v>
       </c>
       <c r="H61" s="8"/>
@@ -42345,7 +42345,7 @@
       <c r="F62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="G62" t="s">
         <v>70</v>
       </c>
       <c r="H62" s="8"/>
@@ -42369,7 +42369,7 @@
       <c r="F63" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="6" t="s">
+      <c r="G63" t="s">
         <v>71</v>
       </c>
       <c r="H63" s="8"/>
@@ -42393,7 +42393,7 @@
       <c r="F64" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G64" t="s">
         <v>72</v>
       </c>
       <c r="H64" s="8"/>
@@ -42417,7 +42417,7 @@
       <c r="F65" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G65" t="s">
         <v>73</v>
       </c>
       <c r="H65" s="8"/>
@@ -42441,7 +42441,7 @@
       <c r="F66" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="G66" t="s">
         <v>74</v>
       </c>
       <c r="H66" s="8"/>
@@ -42465,7 +42465,7 @@
       <c r="F67" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G67" s="6" t="s">
+      <c r="G67" t="s">
         <v>75</v>
       </c>
       <c r="H67" s="8"/>
@@ -42489,7 +42489,7 @@
       <c r="F68" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="G68" t="s">
         <v>76</v>
       </c>
       <c r="H68" s="8"/>
@@ -42513,7 +42513,7 @@
       <c r="F69" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="G69" t="s">
         <v>77</v>
       </c>
       <c r="H69" s="8"/>
@@ -42537,7 +42537,7 @@
       <c r="F70" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G70" t="s">
         <v>78</v>
       </c>
       <c r="H70" s="8"/>
@@ -42561,7 +42561,7 @@
       <c r="F71" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="G71" t="s">
         <v>79</v>
       </c>
       <c r="H71" s="8"/>
@@ -42585,7 +42585,7 @@
       <c r="F72" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G72" s="6" t="s">
+      <c r="G72" t="s">
         <v>80</v>
       </c>
       <c r="H72" s="8"/>
@@ -42609,7 +42609,7 @@
       <c r="F73" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G73" s="6" t="s">
+      <c r="G73" t="s">
         <v>81</v>
       </c>
       <c r="H73" s="8"/>
@@ -42633,7 +42633,7 @@
       <c r="F74" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="G74" t="s">
         <v>82</v>
       </c>
       <c r="H74" s="8"/>
@@ -42657,7 +42657,7 @@
       <c r="F75" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="G75" t="s">
         <v>83</v>
       </c>
       <c r="H75" s="8"/>
@@ -42681,7 +42681,7 @@
       <c r="F76" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G76" s="6" t="s">
+      <c r="G76" t="s">
         <v>84</v>
       </c>
       <c r="H76" s="8"/>
@@ -42705,7 +42705,7 @@
       <c r="F77" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G77" s="6" t="s">
+      <c r="G77" t="s">
         <v>85</v>
       </c>
       <c r="H77" s="8"/>
@@ -42729,7 +42729,7 @@
       <c r="F78" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G78" s="6" t="s">
+      <c r="G78" t="s">
         <v>86</v>
       </c>
       <c r="H78" s="8"/>
@@ -42753,7 +42753,7 @@
       <c r="F79" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G79" s="6" t="s">
+      <c r="G79" t="s">
         <v>87</v>
       </c>
       <c r="H79" s="8"/>
@@ -42777,7 +42777,7 @@
       <c r="F80" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G80" s="6" t="s">
+      <c r="G80" t="s">
         <v>88</v>
       </c>
       <c r="H80" s="8"/>
@@ -42801,7 +42801,7 @@
       <c r="F81" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G81" s="6" t="s">
+      <c r="G81" t="s">
         <v>89</v>
       </c>
       <c r="H81" s="8"/>
@@ -42825,7 +42825,7 @@
       <c r="F82" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G82" s="6" t="s">
+      <c r="G82" t="s">
         <v>90</v>
       </c>
       <c r="H82" s="8"/>
@@ -42849,7 +42849,7 @@
       <c r="F83" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G83" s="6" t="s">
+      <c r="G83" t="s">
         <v>91</v>
       </c>
       <c r="H83" s="8"/>
@@ -42873,7 +42873,7 @@
       <c r="F84" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G84" s="6" t="s">
+      <c r="G84" t="s">
         <v>92</v>
       </c>
       <c r="H84" s="8"/>
@@ -42897,7 +42897,7 @@
       <c r="F85" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="G85" t="s">
         <v>93</v>
       </c>
       <c r="H85" s="8"/>
@@ -42921,7 +42921,7 @@
       <c r="F86" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G86" s="6" t="s">
+      <c r="G86" t="s">
         <v>94</v>
       </c>
       <c r="H86" s="8"/>
@@ -42945,7 +42945,7 @@
       <c r="F87" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G87" s="6" t="s">
+      <c r="G87" t="s">
         <v>95</v>
       </c>
       <c r="H87" s="8"/>
@@ -42969,7 +42969,7 @@
       <c r="F88" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G88" s="6" t="s">
+      <c r="G88" t="s">
         <v>96</v>
       </c>
       <c r="H88" s="8"/>
@@ -42993,7 +42993,7 @@
       <c r="F89" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G89" s="6" t="s">
+      <c r="G89" t="s">
         <v>97</v>
       </c>
       <c r="H89" s="8"/>
@@ -43017,7 +43017,7 @@
       <c r="F90" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G90" s="6" t="s">
+      <c r="G90" t="s">
         <v>98</v>
       </c>
       <c r="H90" s="8"/>
@@ -43041,7 +43041,7 @@
       <c r="F91" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G91" s="6" t="s">
+      <c r="G91" t="s">
         <v>99</v>
       </c>
       <c r="H91" s="8"/>
@@ -43065,7 +43065,7 @@
       <c r="F92" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G92" s="6" t="s">
+      <c r="G92" t="s">
         <v>100</v>
       </c>
       <c r="H92" s="8"/>
@@ -43089,7 +43089,7 @@
       <c r="F93" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G93" s="6" t="s">
+      <c r="G93" t="s">
         <v>101</v>
       </c>
       <c r="H93" s="8"/>
@@ -43113,7 +43113,7 @@
       <c r="F94" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G94" s="6" t="s">
+      <c r="G94" t="s">
         <v>102</v>
       </c>
       <c r="H94" s="8"/>
@@ -43137,7 +43137,7 @@
       <c r="F95" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G95" s="6" t="s">
+      <c r="G95" t="s">
         <v>103</v>
       </c>
       <c r="H95" s="8"/>
@@ -43161,7 +43161,7 @@
       <c r="F96" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G96" s="6" t="s">
+      <c r="G96" t="s">
         <v>104</v>
       </c>
       <c r="H96" s="8"/>
@@ -43185,7 +43185,7 @@
       <c r="F97" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G97" s="6" t="s">
+      <c r="G97" t="s">
         <v>105</v>
       </c>
       <c r="H97" s="8"/>
@@ -43209,7 +43209,7 @@
       <c r="F98" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G98" s="6" t="s">
+      <c r="G98" t="s">
         <v>106</v>
       </c>
       <c r="H98" s="8"/>
@@ -43233,7 +43233,7 @@
       <c r="F99" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G99" s="6" t="s">
+      <c r="G99" t="s">
         <v>107</v>
       </c>
       <c r="H99" s="8"/>
@@ -43257,7 +43257,7 @@
       <c r="F100" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G100" s="6" t="s">
+      <c r="G100" t="s">
         <v>108</v>
       </c>
       <c r="H100" s="8"/>
@@ -43281,7 +43281,7 @@
       <c r="F101" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G101" s="6" t="s">
+      <c r="G101" t="s">
         <v>109</v>
       </c>
       <c r="H101" s="8"/>
@@ -43305,7 +43305,7 @@
       <c r="F102" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G102" s="6" t="s">
+      <c r="G102" t="s">
         <v>110</v>
       </c>
       <c r="H102" s="8"/>
@@ -43329,7 +43329,7 @@
       <c r="F103" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G103" s="6" t="s">
+      <c r="G103" t="s">
         <v>111</v>
       </c>
       <c r="H103" s="8"/>
@@ -43353,7 +43353,7 @@
       <c r="F104" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G104" s="6" t="s">
+      <c r="G104" t="s">
         <v>112</v>
       </c>
       <c r="H104" s="8"/>
@@ -43377,7 +43377,7 @@
       <c r="F105" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G105" s="6" t="s">
+      <c r="G105" t="s">
         <v>113</v>
       </c>
       <c r="H105" s="8"/>
@@ -43401,7 +43401,7 @@
       <c r="F106" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G106" s="6" t="s">
+      <c r="G106" t="s">
         <v>114</v>
       </c>
       <c r="H106" s="8"/>
@@ -43425,7 +43425,7 @@
       <c r="F107" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G107" s="6" t="s">
+      <c r="G107" t="s">
         <v>115</v>
       </c>
       <c r="H107" s="8"/>
@@ -43449,7 +43449,7 @@
       <c r="F108" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G108" s="6" t="s">
+      <c r="G108" t="s">
         <v>116</v>
       </c>
       <c r="H108" s="8"/>
@@ -43473,7 +43473,7 @@
       <c r="F109" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G109" s="6" t="s">
+      <c r="G109" t="s">
         <v>117</v>
       </c>
       <c r="H109" s="8"/>
@@ -43497,7 +43497,7 @@
       <c r="F110" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G110" s="6" t="s">
+      <c r="G110" t="s">
         <v>118</v>
       </c>
       <c r="H110" s="8"/>
@@ -43521,7 +43521,7 @@
       <c r="F111" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G111" s="6" t="s">
+      <c r="G111" t="s">
         <v>119</v>
       </c>
       <c r="H111" s="8"/>
@@ -43545,7 +43545,7 @@
       <c r="F112" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G112" s="6" t="s">
+      <c r="G112" t="s">
         <v>120</v>
       </c>
       <c r="H112" s="8"/>
@@ -43569,7 +43569,7 @@
       <c r="F113" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G113" s="6" t="s">
+      <c r="G113" t="s">
         <v>121</v>
       </c>
       <c r="H113" s="8"/>
@@ -43593,7 +43593,7 @@
       <c r="F114" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G114" s="6" t="s">
+      <c r="G114" t="s">
         <v>122</v>
       </c>
       <c r="H114" s="8"/>
@@ -43617,7 +43617,7 @@
       <c r="F115" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G115" s="6" t="s">
+      <c r="G115" t="s">
         <v>123</v>
       </c>
       <c r="H115" s="8"/>
@@ -43641,7 +43641,7 @@
       <c r="F116" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G116" s="6" t="s">
+      <c r="G116" t="s">
         <v>124</v>
       </c>
       <c r="H116" s="8"/>
@@ -43665,7 +43665,7 @@
       <c r="F117" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G117" s="6" t="s">
+      <c r="G117" t="s">
         <v>125</v>
       </c>
       <c r="H117" s="8"/>
@@ -43689,7 +43689,7 @@
       <c r="F118" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G118" s="6" t="s">
+      <c r="G118" t="s">
         <v>126</v>
       </c>
       <c r="H118" s="8"/>
@@ -43713,7 +43713,7 @@
       <c r="F119" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G119" s="6" t="s">
+      <c r="G119" t="s">
         <v>127</v>
       </c>
       <c r="H119" s="8"/>
@@ -43737,7 +43737,7 @@
       <c r="F120" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G120" s="6" t="s">
+      <c r="G120" t="s">
         <v>128</v>
       </c>
       <c r="H120" s="8"/>
@@ -43761,7 +43761,7 @@
       <c r="F121" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G121" s="6" t="s">
+      <c r="G121" t="s">
         <v>129</v>
       </c>
       <c r="H121" s="8"/>
@@ -43785,7 +43785,7 @@
       <c r="F122" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G122" s="6" t="s">
+      <c r="G122" t="s">
         <v>130</v>
       </c>
       <c r="H122" s="8"/>
@@ -43809,7 +43809,7 @@
       <c r="F123" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G123" s="6" t="s">
+      <c r="G123" t="s">
         <v>131</v>
       </c>
       <c r="H123" s="8"/>
@@ -43833,7 +43833,7 @@
       <c r="F124" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G124" s="6" t="s">
+      <c r="G124" t="s">
         <v>132</v>
       </c>
       <c r="H124" s="8"/>
@@ -43857,7 +43857,7 @@
       <c r="F125" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G125" s="6" t="s">
+      <c r="G125" t="s">
         <v>133</v>
       </c>
       <c r="H125" s="8"/>
@@ -43881,7 +43881,7 @@
       <c r="F126" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G126" s="6" t="s">
+      <c r="G126" t="s">
         <v>134</v>
       </c>
       <c r="H126" s="8"/>
@@ -43905,7 +43905,7 @@
       <c r="F127" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G127" s="6" t="s">
+      <c r="G127" t="s">
         <v>135</v>
       </c>
       <c r="H127" s="8"/>
@@ -43929,7 +43929,7 @@
       <c r="F128" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G128" s="6" t="s">
+      <c r="G128" t="s">
         <v>136</v>
       </c>
       <c r="H128" s="8"/>
@@ -43953,7 +43953,7 @@
       <c r="F129" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G129" s="6" t="s">
+      <c r="G129" t="s">
         <v>137</v>
       </c>
       <c r="H129" s="8"/>
@@ -43977,7 +43977,7 @@
       <c r="F130" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G130" s="6" t="s">
+      <c r="G130" t="s">
         <v>138</v>
       </c>
       <c r="H130" s="8"/>
@@ -44001,7 +44001,7 @@
       <c r="F131" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G131" s="6" t="s">
+      <c r="G131" t="s">
         <v>139</v>
       </c>
       <c r="H131" s="7"/>
@@ -44025,7 +44025,7 @@
       <c r="F132" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G132" s="6" t="s">
+      <c r="G132" t="s">
         <v>140</v>
       </c>
       <c r="H132" s="7"/>
@@ -44049,7 +44049,7 @@
       <c r="F133" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G133" s="6" t="s">
+      <c r="G133" t="s">
         <v>141</v>
       </c>
       <c r="H133" s="7"/>
@@ -44073,7 +44073,7 @@
       <c r="F134" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G134" s="6" t="s">
+      <c r="G134" t="s">
         <v>142</v>
       </c>
       <c r="H134" s="7"/>
@@ -44097,7 +44097,7 @@
       <c r="F135" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G135" s="6" t="s">
+      <c r="G135" t="s">
         <v>143</v>
       </c>
       <c r="H135" s="7"/>
@@ -44121,7 +44121,7 @@
       <c r="F136" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G136" s="6" t="s">
+      <c r="G136" t="s">
         <v>144</v>
       </c>
       <c r="H136" s="7"/>
@@ -44145,7 +44145,7 @@
       <c r="F137" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G137" s="6" t="s">
+      <c r="G137" t="s">
         <v>145</v>
       </c>
       <c r="H137" s="8"/>
@@ -44169,7 +44169,7 @@
       <c r="F138" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G138" s="6" t="s">
+      <c r="G138" t="s">
         <v>146</v>
       </c>
       <c r="H138" s="8"/>
@@ -44193,7 +44193,7 @@
       <c r="F139" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G139" s="6" t="s">
+      <c r="G139" t="s">
         <v>147</v>
       </c>
       <c r="H139" s="8"/>
@@ -44217,7 +44217,7 @@
       <c r="F140" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G140" s="6" t="s">
+      <c r="G140" t="s">
         <v>148</v>
       </c>
       <c r="H140" s="8"/>
@@ -44241,7 +44241,7 @@
       <c r="F141" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G141" s="6" t="s">
+      <c r="G141" t="s">
         <v>149</v>
       </c>
       <c r="H141" s="8"/>
@@ -44265,7 +44265,7 @@
       <c r="F142" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G142" s="6" t="s">
+      <c r="G142" t="s">
         <v>150</v>
       </c>
       <c r="H142" s="8"/>
@@ -44289,7 +44289,7 @@
       <c r="F143" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G143" s="6" t="s">
+      <c r="G143" t="s">
         <v>151</v>
       </c>
       <c r="H143" s="8"/>
@@ -44313,7 +44313,7 @@
       <c r="F144" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G144" s="6" t="s">
+      <c r="G144" t="s">
         <v>152</v>
       </c>
       <c r="H144" s="8"/>
@@ -44337,7 +44337,7 @@
       <c r="F145" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G145" s="6" t="s">
+      <c r="G145" t="s">
         <v>153</v>
       </c>
       <c r="H145" s="8"/>
@@ -44361,7 +44361,7 @@
       <c r="F146" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G146" s="6" t="s">
+      <c r="G146" t="s">
         <v>154</v>
       </c>
       <c r="H146" s="8"/>
@@ -44385,7 +44385,7 @@
       <c r="F147" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G147" s="6" t="s">
+      <c r="G147" t="s">
         <v>155</v>
       </c>
       <c r="H147" s="8"/>
@@ -44409,7 +44409,7 @@
       <c r="F148" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G148" s="6" t="s">
+      <c r="G148" t="s">
         <v>156</v>
       </c>
       <c r="H148" s="8"/>
@@ -44433,7 +44433,7 @@
       <c r="F149" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G149" s="6" t="s">
+      <c r="G149" t="s">
         <v>157</v>
       </c>
       <c r="H149" s="8"/>
@@ -44457,7 +44457,7 @@
       <c r="F150" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G150" s="6" t="s">
+      <c r="G150" t="s">
         <v>158</v>
       </c>
       <c r="H150" s="8"/>
@@ -44481,7 +44481,7 @@
       <c r="F151" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G151" s="6" t="s">
+      <c r="G151" t="s">
         <v>159</v>
       </c>
       <c r="H151" s="8"/>
@@ -44505,7 +44505,7 @@
       <c r="F152" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G152" s="6" t="s">
+      <c r="G152" t="s">
         <v>160</v>
       </c>
       <c r="H152" s="8"/>
@@ -44529,7 +44529,7 @@
       <c r="F153" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G153" s="6" t="s">
+      <c r="G153" t="s">
         <v>161</v>
       </c>
       <c r="H153" s="8"/>
@@ -44553,7 +44553,7 @@
       <c r="F154" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G154" s="6" t="s">
+      <c r="G154" t="s">
         <v>162</v>
       </c>
       <c r="H154" s="8"/>
@@ -44577,7 +44577,7 @@
       <c r="F155" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G155" s="6" t="s">
+      <c r="G155" t="s">
         <v>163</v>
       </c>
       <c r="H155" s="8"/>
@@ -44601,7 +44601,7 @@
       <c r="F156" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G156" s="6" t="s">
+      <c r="G156" t="s">
         <v>164</v>
       </c>
       <c r="H156" s="8"/>
@@ -44625,7 +44625,7 @@
       <c r="F157" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G157" s="6" t="s">
+      <c r="G157" t="s">
         <v>165</v>
       </c>
       <c r="H157" s="8"/>
@@ -44649,7 +44649,7 @@
       <c r="F158" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G158" s="6" t="s">
+      <c r="G158" t="s">
         <v>166</v>
       </c>
       <c r="H158" s="8"/>
@@ -44673,7 +44673,7 @@
       <c r="F159" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="6" t="s">
+      <c r="G159" t="s">
         <v>167</v>
       </c>
       <c r="H159" s="8"/>
@@ -44697,7 +44697,7 @@
       <c r="F160" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G160" s="6" t="s">
+      <c r="G160" t="s">
         <v>168</v>
       </c>
       <c r="H160" s="8"/>
@@ -44721,7 +44721,7 @@
       <c r="F161" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G161" s="6" t="s">
+      <c r="G161" t="s">
         <v>169</v>
       </c>
       <c r="H161" s="8"/>
@@ -44745,7 +44745,7 @@
       <c r="F162" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G162" s="6" t="s">
+      <c r="G162" t="s">
         <v>170</v>
       </c>
       <c r="H162" s="8"/>
@@ -44769,7 +44769,7 @@
       <c r="F163" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G163" s="6" t="s">
+      <c r="G163" t="s">
         <v>171</v>
       </c>
       <c r="H163" s="8"/>
@@ -44793,7 +44793,7 @@
       <c r="F164" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G164" s="6" t="s">
+      <c r="G164" t="s">
         <v>172</v>
       </c>
       <c r="H164" s="8"/>
@@ -44817,7 +44817,7 @@
       <c r="F165" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G165" s="6" t="s">
+      <c r="G165" t="s">
         <v>173</v>
       </c>
       <c r="H165" s="8"/>
@@ -44841,7 +44841,7 @@
       <c r="F166" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G166" s="6" t="s">
+      <c r="G166" t="s">
         <v>174</v>
       </c>
       <c r="H166" s="8"/>
@@ -44865,7 +44865,7 @@
       <c r="F167" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G167" s="6" t="s">
+      <c r="G167" t="s">
         <v>175</v>
       </c>
       <c r="H167" s="8"/>
@@ -44889,7 +44889,7 @@
       <c r="F168" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G168" s="6" t="s">
+      <c r="G168" t="s">
         <v>176</v>
       </c>
       <c r="H168" s="8"/>
@@ -44913,7 +44913,7 @@
       <c r="F169" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G169" s="6" t="s">
+      <c r="G169" t="s">
         <v>177</v>
       </c>
       <c r="H169" s="8"/>
@@ -44937,7 +44937,7 @@
       <c r="F170" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G170" s="6" t="s">
+      <c r="G170" t="s">
         <v>178</v>
       </c>
       <c r="H170" s="8"/>
@@ -44961,7 +44961,7 @@
       <c r="F171" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G171" s="6" t="s">
+      <c r="G171" t="s">
         <v>179</v>
       </c>
       <c r="H171" s="8"/>
@@ -44985,7 +44985,7 @@
       <c r="F172" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G172" s="6" t="s">
+      <c r="G172" t="s">
         <v>180</v>
       </c>
       <c r="H172" s="8"/>
@@ -45009,7 +45009,7 @@
       <c r="F173" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G173" s="6" t="s">
+      <c r="G173" t="s">
         <v>181</v>
       </c>
       <c r="H173" s="8"/>
@@ -45033,7 +45033,7 @@
       <c r="F174" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G174" s="6" t="s">
+      <c r="G174" t="s">
         <v>182</v>
       </c>
       <c r="H174" s="8"/>
@@ -45057,7 +45057,7 @@
       <c r="F175" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G175" s="6" t="s">
+      <c r="G175" t="s">
         <v>183</v>
       </c>
       <c r="H175" s="8"/>
@@ -45081,7 +45081,7 @@
       <c r="F176" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G176" s="6" t="s">
+      <c r="G176" t="s">
         <v>184</v>
       </c>
       <c r="H176" s="8"/>
@@ -45105,7 +45105,7 @@
       <c r="F177" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G177" s="6" t="s">
+      <c r="G177" t="s">
         <v>185</v>
       </c>
       <c r="H177" s="8"/>
@@ -45129,7 +45129,7 @@
       <c r="F178" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G178" s="6" t="s">
+      <c r="G178" t="s">
         <v>186</v>
       </c>
       <c r="H178" s="8"/>
@@ -45153,7 +45153,7 @@
       <c r="F179" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G179" s="6" t="s">
+      <c r="G179" t="s">
         <v>187</v>
       </c>
       <c r="H179" s="8"/>
@@ -45177,7 +45177,7 @@
       <c r="F180" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G180" s="6" t="s">
+      <c r="G180" t="s">
         <v>188</v>
       </c>
       <c r="H180" s="8"/>
@@ -45201,7 +45201,7 @@
       <c r="F181" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G181" s="6" t="s">
+      <c r="G181" t="s">
         <v>189</v>
       </c>
       <c r="H181" s="8"/>
@@ -45225,7 +45225,7 @@
       <c r="F182" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G182" s="6" t="s">
+      <c r="G182" t="s">
         <v>190</v>
       </c>
       <c r="H182" s="8"/>
@@ -45249,7 +45249,7 @@
       <c r="F183" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G183" s="6" t="s">
+      <c r="G183" t="s">
         <v>191</v>
       </c>
       <c r="H183" s="8"/>
@@ -45273,7 +45273,7 @@
       <c r="F184" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G184" s="6" t="s">
+      <c r="G184" t="s">
         <v>192</v>
       </c>
       <c r="H184" s="8"/>
@@ -45297,7 +45297,7 @@
       <c r="F185" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G185" s="6" t="s">
+      <c r="G185" t="s">
         <v>193</v>
       </c>
       <c r="H185" s="8"/>
@@ -45321,7 +45321,7 @@
       <c r="F186" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G186" s="6" t="s">
+      <c r="G186" t="s">
         <v>194</v>
       </c>
       <c r="H186" s="8"/>
@@ -45345,7 +45345,7 @@
       <c r="F187" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G187" s="6" t="s">
+      <c r="G187" t="s">
         <v>195</v>
       </c>
       <c r="H187" s="8"/>
@@ -45369,7 +45369,7 @@
       <c r="F188" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G188" s="6" t="s">
+      <c r="G188" t="s">
         <v>196</v>
       </c>
       <c r="H188" s="8"/>
@@ -45393,7 +45393,7 @@
       <c r="F189" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G189" s="6" t="s">
+      <c r="G189" t="s">
         <v>197</v>
       </c>
       <c r="H189" s="8"/>
@@ -45417,7 +45417,7 @@
       <c r="F190" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G190" s="6" t="s">
+      <c r="G190" t="s">
         <v>198</v>
       </c>
       <c r="H190" s="8"/>
@@ -45441,7 +45441,7 @@
       <c r="F191" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G191" s="6" t="s">
+      <c r="G191" t="s">
         <v>199</v>
       </c>
       <c r="H191" s="8"/>
@@ -45465,7 +45465,7 @@
       <c r="F192" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G192" s="6" t="s">
+      <c r="G192" t="s">
         <v>200</v>
       </c>
       <c r="H192" s="8"/>
@@ -45489,7 +45489,7 @@
       <c r="F193" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G193" s="6" t="s">
+      <c r="G193" t="s">
         <v>201</v>
       </c>
       <c r="H193" s="8"/>
@@ -45513,7 +45513,7 @@
       <c r="F194" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G194" s="6" t="s">
+      <c r="G194" t="s">
         <v>202</v>
       </c>
       <c r="H194" s="8"/>
@@ -45537,7 +45537,7 @@
       <c r="F195" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G195" s="6" t="s">
+      <c r="G195" t="s">
         <v>203</v>
       </c>
       <c r="H195" s="8"/>
@@ -45561,7 +45561,7 @@
       <c r="F196" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G196" s="6" t="s">
+      <c r="G196" t="s">
         <v>204</v>
       </c>
       <c r="H196" s="8"/>
@@ -45585,7 +45585,7 @@
       <c r="F197" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G197" s="6" t="s">
+      <c r="G197" t="s">
         <v>205</v>
       </c>
       <c r="H197" s="8"/>
@@ -45609,7 +45609,7 @@
       <c r="F198" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G198" s="6" t="s">
+      <c r="G198" t="s">
         <v>206</v>
       </c>
       <c r="H198" s="8"/>
@@ -45633,7 +45633,7 @@
       <c r="F199" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G199" s="6" t="s">
+      <c r="G199" t="s">
         <v>207</v>
       </c>
       <c r="H199" s="8"/>
@@ -45657,7 +45657,7 @@
       <c r="F200" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G200" s="6" t="s">
+      <c r="G200" t="s">
         <v>208</v>
       </c>
       <c r="H200" s="8"/>
@@ -45681,7 +45681,7 @@
       <c r="F201" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G201" s="6" t="s">
+      <c r="G201" t="s">
         <v>209</v>
       </c>
       <c r="H201" s="8"/>
@@ -45705,7 +45705,7 @@
       <c r="F202" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G202" s="6" t="s">
+      <c r="G202" t="s">
         <v>210</v>
       </c>
       <c r="H202" s="8"/>
@@ -45729,7 +45729,7 @@
       <c r="F203" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G203" s="6" t="s">
+      <c r="G203" t="s">
         <v>211</v>
       </c>
       <c r="H203" s="8"/>
@@ -45753,7 +45753,7 @@
       <c r="F204" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G204" s="6" t="s">
+      <c r="G204" t="s">
         <v>212</v>
       </c>
       <c r="H204" s="8"/>
@@ -45777,7 +45777,7 @@
       <c r="F205" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G205" s="6" t="s">
+      <c r="G205" t="s">
         <v>213</v>
       </c>
       <c r="H205" s="8"/>
@@ -45801,7 +45801,7 @@
       <c r="F206" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G206" s="6" t="s">
+      <c r="G206" t="s">
         <v>214</v>
       </c>
       <c r="H206" s="8"/>
@@ -45825,7 +45825,7 @@
       <c r="F207" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G207" s="6" t="s">
+      <c r="G207" t="s">
         <v>215</v>
       </c>
       <c r="H207" s="8"/>
@@ -45849,7 +45849,7 @@
       <c r="F208" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G208" s="6" t="s">
+      <c r="G208" t="s">
         <v>216</v>
       </c>
       <c r="H208" s="8"/>
@@ -45873,7 +45873,7 @@
       <c r="F209" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G209" s="6" t="s">
+      <c r="G209" t="s">
         <v>217</v>
       </c>
       <c r="H209" s="8"/>
@@ -45897,7 +45897,7 @@
       <c r="F210" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G210" s="6" t="s">
+      <c r="G210" t="s">
         <v>218</v>
       </c>
       <c r="H210" s="8"/>
@@ -45921,7 +45921,7 @@
       <c r="F211" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G211" s="6" t="s">
+      <c r="G211" t="s">
         <v>219</v>
       </c>
       <c r="H211" s="8"/>
@@ -45945,7 +45945,7 @@
       <c r="F212" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G212" s="6" t="s">
+      <c r="G212" t="s">
         <v>220</v>
       </c>
       <c r="H212" s="8"/>
@@ -45969,7 +45969,7 @@
       <c r="F213" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G213" s="6" t="s">
+      <c r="G213" t="s">
         <v>221</v>
       </c>
       <c r="H213" s="8"/>
@@ -45993,7 +45993,7 @@
       <c r="F214" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G214" s="6" t="s">
+      <c r="G214" t="s">
         <v>222</v>
       </c>
       <c r="H214" s="8"/>
@@ -46017,7 +46017,7 @@
       <c r="F215" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G215" s="6" t="s">
+      <c r="G215" t="s">
         <v>223</v>
       </c>
       <c r="H215" s="8"/>
@@ -46041,7 +46041,7 @@
       <c r="F216" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G216" s="6" t="s">
+      <c r="G216" t="s">
         <v>224</v>
       </c>
       <c r="H216" s="8"/>
@@ -46065,7 +46065,7 @@
       <c r="F217" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G217" s="6" t="s">
+      <c r="G217" t="s">
         <v>225</v>
       </c>
       <c r="H217" s="8"/>
@@ -46089,7 +46089,7 @@
       <c r="F218" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G218" s="6" t="s">
+      <c r="G218" t="s">
         <v>226</v>
       </c>
       <c r="H218" s="8"/>
@@ -46113,7 +46113,7 @@
       <c r="F219" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G219" s="6" t="s">
+      <c r="G219" t="s">
         <v>227</v>
       </c>
       <c r="H219" s="8"/>
@@ -46137,7 +46137,7 @@
       <c r="F220" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G220" s="6" t="s">
+      <c r="G220" t="s">
         <v>228</v>
       </c>
       <c r="H220" s="8"/>
@@ -46161,7 +46161,7 @@
       <c r="F221" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G221" s="6" t="s">
+      <c r="G221" t="s">
         <v>229</v>
       </c>
       <c r="H221" s="8"/>
@@ -46185,7 +46185,7 @@
       <c r="F222" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G222" s="6" t="s">
+      <c r="G222" t="s">
         <v>230</v>
       </c>
       <c r="H222" s="8"/>
@@ -46209,7 +46209,7 @@
       <c r="F223" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G223" s="6" t="s">
+      <c r="G223" t="s">
         <v>231</v>
       </c>
       <c r="H223" s="8"/>
@@ -46233,7 +46233,7 @@
       <c r="F224" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G224" s="6" t="s">
+      <c r="G224" t="s">
         <v>232</v>
       </c>
       <c r="H224" s="8"/>
@@ -46257,7 +46257,7 @@
       <c r="F225" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G225" s="6" t="s">
+      <c r="G225" t="s">
         <v>233</v>
       </c>
       <c r="H225" s="8"/>
@@ -46281,7 +46281,7 @@
       <c r="F226" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G226" s="6" t="s">
+      <c r="G226" t="s">
         <v>234</v>
       </c>
       <c r="H226" s="8"/>
@@ -46305,7 +46305,7 @@
       <c r="F227" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G227" s="6" t="s">
+      <c r="G227" t="s">
         <v>235</v>
       </c>
       <c r="H227" s="8"/>
@@ -46329,7 +46329,7 @@
       <c r="F228" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G228" s="6" t="s">
+      <c r="G228" t="s">
         <v>236</v>
       </c>
       <c r="H228" s="8"/>
@@ -46353,7 +46353,7 @@
       <c r="F229" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G229" s="6" t="s">
+      <c r="G229" t="s">
         <v>237</v>
       </c>
       <c r="H229" s="8"/>
@@ -46377,7 +46377,7 @@
       <c r="F230" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G230" s="6" t="s">
+      <c r="G230" t="s">
         <v>238</v>
       </c>
       <c r="H230" s="8"/>
@@ -46401,7 +46401,7 @@
       <c r="F231" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G231" s="6" t="s">
+      <c r="G231" t="s">
         <v>239</v>
       </c>
       <c r="H231" s="8"/>
@@ -46425,7 +46425,7 @@
       <c r="F232" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G232" s="6" t="s">
+      <c r="G232" t="s">
         <v>240</v>
       </c>
       <c r="H232" s="8"/>
@@ -46449,7 +46449,7 @@
       <c r="F233" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G233" s="6" t="s">
+      <c r="G233" t="s">
         <v>241</v>
       </c>
       <c r="H233" s="8"/>
@@ -46473,7 +46473,7 @@
       <c r="F234" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G234" s="6" t="s">
+      <c r="G234" t="s">
         <v>242</v>
       </c>
       <c r="H234" s="8"/>
@@ -46497,7 +46497,7 @@
       <c r="F235" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G235" s="6" t="s">
+      <c r="G235" t="s">
         <v>243</v>
       </c>
       <c r="H235" s="8"/>
@@ -46521,7 +46521,7 @@
       <c r="F236" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G236" s="6" t="s">
+      <c r="G236" t="s">
         <v>244</v>
       </c>
       <c r="H236" s="8"/>
@@ -46545,7 +46545,7 @@
       <c r="F237" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G237" s="6" t="s">
+      <c r="G237" t="s">
         <v>245</v>
       </c>
       <c r="H237" s="8"/>
@@ -46569,7 +46569,7 @@
       <c r="F238" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G238" s="6" t="s">
+      <c r="G238" t="s">
         <v>246</v>
       </c>
       <c r="H238" s="8"/>
@@ -46593,7 +46593,7 @@
       <c r="F239" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G239" s="6" t="s">
+      <c r="G239" t="s">
         <v>247</v>
       </c>
       <c r="H239" s="8"/>
@@ -46617,7 +46617,7 @@
       <c r="F240" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G240" s="6" t="s">
+      <c r="G240" t="s">
         <v>248</v>
       </c>
       <c r="H240" s="8"/>
@@ -46641,7 +46641,7 @@
       <c r="F241" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G241" s="6" t="s">
+      <c r="G241" t="s">
         <v>249</v>
       </c>
       <c r="H241" s="8"/>
@@ -46665,7 +46665,7 @@
       <c r="F242" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G242" s="6" t="s">
+      <c r="G242" t="s">
         <v>250</v>
       </c>
       <c r="H242" s="8"/>
@@ -46689,7 +46689,7 @@
       <c r="F243" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G243" s="6" t="s">
+      <c r="G243" t="s">
         <v>251</v>
       </c>
       <c r="H243" s="8"/>
@@ -46713,7 +46713,7 @@
       <c r="F244" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G244" s="6" t="s">
+      <c r="G244" t="s">
         <v>252</v>
       </c>
       <c r="H244" s="8"/>
@@ -46737,7 +46737,7 @@
       <c r="F245" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G245" s="6" t="s">
+      <c r="G245" t="s">
         <v>253</v>
       </c>
       <c r="H245" s="8"/>
@@ -46761,7 +46761,7 @@
       <c r="F246" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G246" s="6" t="s">
+      <c r="G246" t="s">
         <v>254</v>
       </c>
       <c r="H246" s="8"/>
@@ -46785,7 +46785,7 @@
       <c r="F247" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G247" s="6" t="s">
+      <c r="G247" t="s">
         <v>255</v>
       </c>
       <c r="H247" s="8"/>
@@ -46809,7 +46809,7 @@
       <c r="F248" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G248" s="6" t="s">
+      <c r="G248" t="s">
         <v>256</v>
       </c>
       <c r="H248" s="8"/>
@@ -46833,7 +46833,7 @@
       <c r="F249" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G249" s="6" t="s">
+      <c r="G249" t="s">
         <v>257</v>
       </c>
       <c r="H249" s="8"/>
@@ -46857,7 +46857,7 @@
       <c r="F250" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G250" s="6" t="s">
+      <c r="G250" t="s">
         <v>258</v>
       </c>
       <c r="H250" s="8"/>
@@ -46881,7 +46881,7 @@
       <c r="F251" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G251" s="6" t="s">
+      <c r="G251" t="s">
         <v>259</v>
       </c>
       <c r="H251" s="8"/>
@@ -46905,7 +46905,7 @@
       <c r="F252" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G252" s="6" t="s">
+      <c r="G252" t="s">
         <v>260</v>
       </c>
       <c r="H252" s="8"/>
@@ -46929,7 +46929,7 @@
       <c r="F253" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G253" s="6" t="s">
+      <c r="G253" t="s">
         <v>261</v>
       </c>
       <c r="H253" s="8"/>
@@ -46953,7 +46953,7 @@
       <c r="F254" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G254" s="6" t="s">
+      <c r="G254" t="s">
         <v>262</v>
       </c>
       <c r="H254" s="8"/>
@@ -46977,7 +46977,7 @@
       <c r="F255" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G255" s="6" t="s">
+      <c r="G255" t="s">
         <v>263</v>
       </c>
       <c r="H255" s="8"/>
@@ -47001,7 +47001,7 @@
       <c r="F256" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G256" s="6" t="s">
+      <c r="G256" t="s">
         <v>264</v>
       </c>
       <c r="H256" s="8"/>
@@ -47025,7 +47025,7 @@
       <c r="F257" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G257" s="6" t="s">
+      <c r="G257" t="s">
         <v>265</v>
       </c>
       <c r="H257" s="8"/>
@@ -47049,7 +47049,7 @@
       <c r="F258" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G258" s="6" t="s">
+      <c r="G258" t="s">
         <v>266</v>
       </c>
       <c r="H258" s="8"/>
@@ -47073,7 +47073,7 @@
       <c r="F259" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G259" s="6" t="s">
+      <c r="G259" t="s">
         <v>267</v>
       </c>
       <c r="H259" s="8"/>
@@ -47097,7 +47097,7 @@
       <c r="F260" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G260" s="6" t="s">
+      <c r="G260" t="s">
         <v>268</v>
       </c>
       <c r="H260" s="8"/>
@@ -47121,7 +47121,7 @@
       <c r="F261" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G261" s="6" t="s">
+      <c r="G261" t="s">
         <v>269</v>
       </c>
       <c r="H261" s="8"/>
@@ -47145,7 +47145,7 @@
       <c r="F262" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G262" s="6" t="s">
+      <c r="G262" t="s">
         <v>270</v>
       </c>
       <c r="H262" s="8"/>
@@ -47169,7 +47169,7 @@
       <c r="F263" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G263" s="6" t="s">
+      <c r="G263" t="s">
         <v>271</v>
       </c>
       <c r="H263" s="8"/>
@@ -47193,7 +47193,7 @@
       <c r="F264" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G264" s="6" t="s">
+      <c r="G264" t="s">
         <v>272</v>
       </c>
       <c r="H264" s="8"/>
@@ -47217,7 +47217,7 @@
       <c r="F265" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G265" s="6" t="s">
+      <c r="G265" t="s">
         <v>273</v>
       </c>
       <c r="H265" s="8"/>
@@ -47241,7 +47241,7 @@
       <c r="F266" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G266" s="6" t="s">
+      <c r="G266" t="s">
         <v>274</v>
       </c>
       <c r="H266" s="8"/>
@@ -47265,7 +47265,7 @@
       <c r="F267" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G267" s="6" t="s">
+      <c r="G267" t="s">
         <v>275</v>
       </c>
       <c r="H267" s="8"/>
@@ -47289,7 +47289,7 @@
       <c r="F268" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G268" s="6" t="s">
+      <c r="G268" t="s">
         <v>276</v>
       </c>
       <c r="H268" s="8"/>
@@ -47313,7 +47313,7 @@
       <c r="F269" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G269" s="6" t="s">
+      <c r="G269" t="s">
         <v>277</v>
       </c>
       <c r="H269" s="8"/>
@@ -47337,7 +47337,7 @@
       <c r="F270" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G270" s="6" t="s">
+      <c r="G270" t="s">
         <v>278</v>
       </c>
       <c r="H270" s="8"/>
@@ -47361,7 +47361,7 @@
       <c r="F271" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G271" s="6" t="s">
+      <c r="G271" t="s">
         <v>279</v>
       </c>
       <c r="H271" s="8"/>
@@ -47385,7 +47385,7 @@
       <c r="F272" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G272" s="6" t="s">
+      <c r="G272" t="s">
         <v>280</v>
       </c>
       <c r="H272" s="8"/>
@@ -47409,7 +47409,7 @@
       <c r="F273" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G273" s="6" t="s">
+      <c r="G273" t="s">
         <v>281</v>
       </c>
       <c r="H273" s="8"/>
@@ -47433,7 +47433,7 @@
       <c r="F274" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G274" s="6" t="s">
+      <c r="G274" t="s">
         <v>282</v>
       </c>
       <c r="H274" s="8"/>
@@ -47457,7 +47457,7 @@
       <c r="F275" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G275" s="6" t="s">
+      <c r="G275" t="s">
         <v>283</v>
       </c>
       <c r="H275" s="8"/>

</xml_diff>